<commit_message>
Data Processing into multiple subsheets
</commit_message>
<xml_diff>
--- a/public/excel_files/grouped_data.xlsx
+++ b/public/excel_files/grouped_data.xlsx
@@ -4,6 +4,11 @@
   <workbookPr date1904="false"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -363,176 +368,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:A46"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <dimension ref="A1:E8"/>
   <sheetData>
-    <row r="1" spans="1:1" customFormat="false">
+    <row r="1" spans="1:5" customFormat="false">
       <c r="A1" s="0" t="str">
-        <v>Category: 307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" customFormat="false">
-      <c r="A2" s="0" t="str">
-        <v>Comment: There were some points in the class where the sheer number of assignments given out made it unclear what was expected.</v>
+        <v>Based on what the instructor(s) communicated, and the information provided in the course syllabus, I understood what was expected of me.</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <v>Perfect Score</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>Average</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>Median</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>Mode</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0">
+        <v>2.4375</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>2.0</v>
       </c>
     </row>
     <row r="3" spans="1:1" customFormat="false">
       <c r="A3" s="0" t="str">
-        <v>Comment: The requirements for some assignments were vague and sometimes I feel that some requirements weren't conveyed well to us.</v>
+        <v>There were some points in the class where the sheer number of assignments given out made it unclear what was expected.</v>
       </c>
     </row>
     <row r="4" spans="1:1" customFormat="false">
       <c r="A4" s="0" t="str">
-        <v>Comment: A lot of the project requirements and document requirements were confusing because the rubric was not provided in the Canvas assignments</v>
+        <v>The requirements for some assignments were vague and sometimes I feel that some requirements weren't conveyed well to us.</v>
       </c>
     </row>
     <row r="5" spans="1:1" customFormat="false">
       <c r="A5" s="0" t="str">
-        <v>Comment: There is so much information on the syllabus and Canvas that there is a bit of overload, complicating what exactly I should be prioritizing in the class</v>
+        <v>A lot of the project requirements and document requirements were confusing because the rubric was not provided in the Canvas assignments</v>
       </c>
     </row>
     <row r="6" spans="1:1" customFormat="false">
       <c r="A6" s="0" t="str">
-        <v>Comment: I think there were organization issues but it was fixed towards the middle</v>
+        <v>There is so much information on the syllabus and Canvas that there is a bit of overload, complicating what exactly I should be prioritizing in the class</v>
       </c>
     </row>
     <row r="7" spans="1:1" customFormat="false">
       <c r="A7" s="0" t="str">
-        <v>Comment: While it was clear for the most part, the way the course was structured was confusing</v>
+        <v>I think there were organization issues but it was fixed towards the middle</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" customFormat="false">
+      <c r="A8" s="0" t="str">
+        <v>While it was clear for the most part, the way the course was structured was confusing</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <dimension ref="A1:E3"/>
+  <sheetData>
+    <row r="1" spans="1:5" customFormat="false">
+      <c r="A1" s="0" t="str">
+        <v>Feedback in this course helped me learn. Please note, feedback can be either informal (e.g., in class discussion, chat boards, think-pair-share, office hour discussions, help sessions) or formal (e.g., written or clinical assessments, review of exams, peer reviews, clicker questions).</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <v>Perfect Score</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>Average</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>Median</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>Mode</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="D2" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="E2" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>The sprint audits were helpful in ensuring we were on track, but it felt like a lot of times we were simply quizzed on random topics (ie fat vs skinny models) that weren't really discussed much in class.</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <dimension ref="A1:E9"/>
+  <sheetData>
+    <row r="1" spans="1:5" customFormat="false">
+      <c r="A1" s="0" t="str">
+        <v>Please rate the organization of this course.</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <v>Perfect Score</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>Average</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>Median</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>Mode</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0">
+        <v>2.4375</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>It felt much more organized toward the middle/end of the semester, but the beginning felt a bit unorganized in terms of lectures and assignments.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" customFormat="false">
+      <c r="A4" s="0" t="str">
+        <v>While the canvas modules themselves were technically organized, expectations for assignments especially near the beginning of the class were rather unclear with regards to grading. Even though the project notebook for example and the lesson plan were released at the beginning of the course for us to access and read through at any time, the amount of content was far too overwhelming to really understand all the minute details that were expected. Sprint 1 in particular I did not really enjoy because even though it served as a learning experience I think it would have been far more useful to not just let us all deal with it and basically experience failure to learn. I think going over each assignment and aspects of the project notebook in more detail especially early on and emphasizing relevant points can set students up better for success earlier.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" customFormat="false">
+      <c r="A5" s="0" t="str">
+        <v>I wish the assignments and submission for the assignments were done more through Canvas and not through Teams. There was a case in which I renamed a Teams file for submission, and that changed the timestamp for modification. My team lost credit for this assignment because of this, even though we technically submitted the original file on time. If the submission was done through Canvas then this wouldn't have been an issue.</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" customFormat="false">
+      <c r="A6" s="0" t="str">
+        <v>Many assignments are uploaded last minute, making it hard to plan ahead. Many assignments have very broad rubrics, so when we turn an an assignment we get told we have to change a bunch of stuff even though the assignment never specified it. Many assignments have conflicting instructions and dead links to further details.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" customFormat="false">
+      <c r="A7" s="0" t="str">
+        <v>There was just too much information consolidated in one place with the excel rubrics. It made it a chore to go through.</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" customFormat="false">
+      <c r="A8" s="0" t="str">
+        <v>There were too much to keep track of. You would always miss something.</v>
       </c>
     </row>
     <row r="9" spans="1:1" customFormat="false">
       <c r="A9" s="0" t="str">
-        <v>Category: 297</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" customFormat="false">
-      <c r="A11" s="0" t="str">
-        <v>Category: 315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" customFormat="false">
-      <c r="A13" s="0" t="str">
-        <v>Category: 311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" customFormat="false">
-      <c r="A14" s="0" t="str">
-        <v>Comment: The sprint audits were helpful in ensuring we were on track, but it felt like a lot of times we were simply quizzed on random topics (ie fat vs skinny models) that weren't really discussed much in class.</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" customFormat="false">
-      <c r="A16" s="0" t="str">
-        <v>Category: 300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" customFormat="false">
-      <c r="A18" s="0" t="str">
-        <v>Category: 302</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" customFormat="false">
-      <c r="A20" s="0" t="str">
-        <v>Category: 313</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" customFormat="false">
-      <c r="A22" s="0" t="str">
-        <v>Category: 4287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" customFormat="false">
-      <c r="A24" s="0" t="str">
-        <v>Category: 301</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" customFormat="false">
-      <c r="A25" s="0" t="str">
-        <v>Comment: It felt much more organized toward the middle/end of the semester, but the beginning felt a bit unorganized in terms of lectures and assignments.</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" customFormat="false">
-      <c r="A26" s="0" t="str">
-        <v>Comment: While the canvas modules themselves were technically organized, expectations for assignments especially near the beginning of the class were rather unclear with regards to grading. Even though the project notebook for example and the lesson plan were released at the beginning of the course for us to access and read through at any time, the amount of content was far too overwhelming to really understand all the minute details that were expected. Sprint 1 in particular I did not really enjoy because even though it served as a learning experience I think it would have been far more useful to not just let us all deal with it and basically experience failure to learn. I think going over each assignment and aspects of the project notebook in more detail especially early on and emphasizing relevant points can set students up better for success earlier.</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" customFormat="false">
-      <c r="A27" s="0" t="str">
-        <v>Comment: I wish the assignments and submission for the assignments were done more through Canvas and not through Teams. There was a case in which I renamed a Teams file for submission, and that changed the timestamp for modification. My team lost credit for this assignment because of this, even though we technically submitted the original file on time. If the submission was done through Canvas then this wouldn't have been an issue.</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" customFormat="false">
-      <c r="A28" s="0" t="str">
-        <v>Comment: Many assignments are uploaded last minute, making it hard to plan ahead. Many assignments have very broad rubrics, so when we turn an an assignment we get told we have to change a bunch of stuff even though the assignment never specified it. Many assignments have conflicting instructions and dead links to further details.</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" customFormat="false">
-      <c r="A29" s="0" t="str">
-        <v>Comment: There was just too much information consolidated in one place with the excel rubrics. It made it a chore to go through.</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" customFormat="false">
-      <c r="A30" s="0" t="str">
-        <v>Comment: There were too much to keep track of. You would always miss something.</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" customFormat="false">
-      <c r="A31" s="0" t="str">
-        <v>Comment: There are way too many assignments. It's genuinely difficult to keep up sometimes because there are so many.</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" customFormat="false">
-      <c r="A33" s="0" t="str">
-        <v>Category: 318</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" customFormat="false">
-      <c r="A35" s="0" t="str">
-        <v>Category: 316</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" customFormat="false">
-      <c r="A36" s="0" t="str">
-        <v>Comment: Professor Wade is always open to feedback and any questions</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" customFormat="false">
-      <c r="A37" s="0" t="str">
-        <v>Comment: Very helpful with specific questions</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" customFormat="false">
-      <c r="A38" s="0" t="str">
-        <v>Comment: Again, the sheer amount of assignments combined with the overwhelming documentation was just painful. It made coming to lecture a chore because there was almost always more than one participation activity that couldn't even be completed in class because of the amount of time it took.</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" customFormat="false">
-      <c r="A40" s="0" t="str">
-        <v>Category: 317</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" customFormat="false">
-      <c r="A42" s="0" t="str">
-        <v>Category: 308</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" customFormat="false">
-      <c r="A43" s="0" t="str">
-        <v>Comment: After the first couple weeks learning the basics of Ruby on Rails I felt like we were just thrown on our own to complete weekly labs and work on the team project. We were usually forced to figure stuff out on our own at that point. While the lectures covered the concepts I did not really feel like they covered relevant application of what we learned aside from the participation quizzes which were sometimes just completely separate from the actual lecture content of the day.</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" customFormat="false">
-      <c r="A44" s="0" t="str">
-        <v>Comment: Initially we had some learning for Ruby on Rails but after it was pretty much on us to learn after this. Other skills, such as documentation and project management were expected but not really well taught.</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" customFormat="false">
-      <c r="A45" s="0" t="str">
-        <v>Comment: I learned many technical skills in Rails and project development</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" customFormat="false">
-      <c r="A46" s="0" t="str">
-        <v>Comment: I am not the biggest fan of rails</v>
+        <v>There are way too many assignments. It's genuinely difficult to keep up sometimes because there are so many.</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <dimension ref="A1:E5"/>
+  <sheetData>
+    <row r="1" spans="1:5" customFormat="false">
+      <c r="A1" s="0" t="str">
+        <v>The instructor fostered an effective learning environment.</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <v>Perfect Score</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>Average</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>Median</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>Mode</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>Professor Wade is always open to feedback and any questions</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" customFormat="false">
+      <c r="A4" s="0" t="str">
+        <v>Very helpful with specific questions</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" customFormat="false">
+      <c r="A5" s="0" t="str">
+        <v>Again, the sheer amount of assignments combined with the overwhelming documentation was just painful. It made coming to lecture a chore because there was almost always more than one participation activity that couldn't even be completed in class because of the amount of time it took.</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <dimension ref="A1:E6"/>
+  <sheetData>
+    <row r="1" spans="1:5" customFormat="false">
+      <c r="A1" s="0" t="str">
+        <v>This course helped me learn concepts or skills as stated in course objectives/outcomes.</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <v>Perfect Score</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>Average</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>Median</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>Mode</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0">
+        <v>3.3125</v>
+      </c>
+      <c r="D2" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>After the first couple weeks learning the basics of Ruby on Rails I felt like we were just thrown on our own to complete weekly labs and work on the team project. We were usually forced to figure stuff out on our own at that point. While the lectures covered the concepts I did not really feel like they covered relevant application of what we learned aside from the participation quizzes which were sometimes just completely separate from the actual lecture content of the day.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" customFormat="false">
+      <c r="A4" s="0" t="str">
+        <v>Initially we had some learning for Ruby on Rails but after it was pretty much on us to learn after this. Other skills, such as documentation and project management were expected but not really well taught.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" customFormat="false">
+      <c r="A5" s="0" t="str">
+        <v>I learned many technical skills in Rails and project development</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" customFormat="false">
+      <c r="A6" s="0" t="str">
+        <v>I am not the biggest fan of rails</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Processing Uploaded file and Rspec coverage
</commit_message>
<xml_diff>
--- a/public/excel_files/grouped_data.xlsx
+++ b/public/excel_files/grouped_data.xlsx
@@ -3,12 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="Question 11" sheetId="1" r:id="rId3"/>
+    <sheet name="Question 12" sheetId="2" r:id="rId4"/>
+    <sheet name="Question 13" sheetId="3" r:id="rId5"/>
+    <sheet name="Question 14" sheetId="4" r:id="rId6"/>
+    <sheet name="Question 15" sheetId="5" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -368,12 +367,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E8"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
@@ -441,7 +434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E3"/>
   <sheetData>
@@ -485,7 +478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E9"/>
   <sheetData>
@@ -559,7 +552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E5"/>
   <sheetData>
@@ -613,7 +606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E6"/>
   <sheetData>

</xml_diff>